<commit_message>
Zafer Bey'in hikayesi metin biçimlendirme: satır sonları düzeltildi, paragraflar iyileştirildi
</commit_message>
<xml_diff>
--- a/static/sonuclar.xlsx
+++ b/static/sonuclar.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q132"/>
+  <dimension ref="A1:Q136"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7528,6 +7528,274 @@
         </is>
       </c>
     </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2025-08-05 11:34</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Hacer Yaren Ünsal</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>Hacer Yaren Ünsal</t>
+        </is>
+      </c>
+      <c r="D133" t="n">
+        <v>24</v>
+      </c>
+      <c r="E133" t="n">
+        <v>26</v>
+      </c>
+      <c r="F133" t="n">
+        <v>20</v>
+      </c>
+      <c r="G133" t="n">
+        <v>26</v>
+      </c>
+      <c r="H133" t="n">
+        <v>25</v>
+      </c>
+      <c r="I133" t="n">
+        <v>23</v>
+      </c>
+      <c r="J133" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="K133" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="L133" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="M133" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="N133" t="inlineStr">
+        <is>
+          <t>%24.96</t>
+        </is>
+      </c>
+      <c r="O133" t="inlineStr">
+        <is>
+          <t>%27.13</t>
+        </is>
+      </c>
+      <c r="P133" t="inlineStr">
+        <is>
+          <t>%22.96</t>
+        </is>
+      </c>
+      <c r="Q133" t="inlineStr">
+        <is>
+          <t>%24.96</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2025-08-05 11:44</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Hacer Yaren Ünsal</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>Hacer Yaren Ünsal</t>
+        </is>
+      </c>
+      <c r="D134" t="n">
+        <v>24</v>
+      </c>
+      <c r="E134" t="n">
+        <v>22</v>
+      </c>
+      <c r="F134" t="n">
+        <v>16</v>
+      </c>
+      <c r="G134" t="n">
+        <v>21</v>
+      </c>
+      <c r="H134" t="n">
+        <v>23</v>
+      </c>
+      <c r="I134" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="J134" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="K134" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="L134" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="M134" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="N134" t="inlineStr">
+        <is>
+          <t>%18.47</t>
+        </is>
+      </c>
+      <c r="O134" t="inlineStr">
+        <is>
+          <t>%29.45</t>
+        </is>
+      </c>
+      <c r="P134" t="inlineStr">
+        <is>
+          <t>%20.07</t>
+        </is>
+      </c>
+      <c r="Q134" t="inlineStr">
+        <is>
+          <t>%32.01</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2025-08-05 11:51</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Hacer Yaren Ünsal</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>Hacer Yaren Ünsal</t>
+        </is>
+      </c>
+      <c r="D135" t="n">
+        <v>24</v>
+      </c>
+      <c r="E135" t="n">
+        <v>33</v>
+      </c>
+      <c r="F135" t="n">
+        <v>29</v>
+      </c>
+      <c r="G135" t="n">
+        <v>29</v>
+      </c>
+      <c r="H135" t="n">
+        <v>28.5</v>
+      </c>
+      <c r="I135" t="n">
+        <v>29</v>
+      </c>
+      <c r="J135" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="K135" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="L135" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M135" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="N135" t="inlineStr">
+        <is>
+          <t>%35.87</t>
+        </is>
+      </c>
+      <c r="O135" t="inlineStr">
+        <is>
+          <t>%23.5</t>
+        </is>
+      </c>
+      <c r="P135" t="inlineStr">
+        <is>
+          <t>%24.54</t>
+        </is>
+      </c>
+      <c r="Q135" t="inlineStr">
+        <is>
+          <t>%16.08</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2025-08-07 13:58</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>yaren</t>
+        </is>
+      </c>
+      <c r="D136" t="n">
+        <v>24</v>
+      </c>
+      <c r="E136" t="n">
+        <v>21</v>
+      </c>
+      <c r="F136" t="n">
+        <v>23</v>
+      </c>
+      <c r="G136" t="n">
+        <v>18</v>
+      </c>
+      <c r="H136" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="I136" t="n">
+        <v>20.5</v>
+      </c>
+      <c r="J136" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="K136" t="n">
+        <v>0.27</v>
+      </c>
+      <c r="L136" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="M136" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="N136" t="inlineStr">
+        <is>
+          <t>%20.02</t>
+        </is>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>%26.86</t>
+        </is>
+      </c>
+      <c r="P136" t="inlineStr">
+        <is>
+          <t>%22.69</t>
+        </is>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>%30.44</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>